<commit_message>
signals in object only to be called with eval when needed
</commit_message>
<xml_diff>
--- a/inputVars.xlsx
+++ b/inputVars.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="992" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
@@ -359,7 +359,7 @@
   <dimension ref="B4:G23"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I11" activeCellId="0" sqref="I11"/>
+      <selection pane="topLeft" activeCell="H21" activeCellId="0" sqref="H21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -618,7 +618,9 @@
       <c r="D17" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="E17" s="1"/>
+      <c r="E17" s="1" t="n">
+        <v>10</v>
+      </c>
       <c r="F17" s="3" t="n">
         <v>0.05</v>
       </c>
@@ -626,7 +628,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="E21" s="5" t="s">
         <v>33</v>
       </c>

</xml_diff>

<commit_message>
with price above and below operations
</commit_message>
<xml_diff>
--- a/inputVars.xlsx
+++ b/inputVars.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="54">
   <si>
     <t>Signal Name</t>
   </si>
@@ -216,6 +216,60 @@
       </rPr>
       <t>to that day </t>
     </r>
+  </si>
+  <si>
+    <t>Section 3</t>
+  </si>
+  <si>
+    <t>operation</t>
+  </si>
+  <si>
+    <t>signal</t>
+  </si>
+  <si>
+    <t>Col 1</t>
+  </si>
+  <si>
+    <t>variable crossPercent 3</t>
+  </si>
+  <si>
+    <t>Col 2</t>
+  </si>
+  <si>
+    <t>crossAbove 10 50</t>
+  </si>
+  <si>
+    <t>crossAbove 10 100</t>
+  </si>
+  <si>
+    <t>crossAbove 10 200</t>
+  </si>
+  <si>
+    <t>Col 3</t>
+  </si>
+  <si>
+    <t>topLine 10</t>
+  </si>
+  <si>
+    <t>Col 4</t>
+  </si>
+  <si>
+    <t>Col 5</t>
+  </si>
+  <si>
+    <t>Col 6</t>
+  </si>
+  <si>
+    <t>Col 7</t>
+  </si>
+  <si>
+    <t>Col 8</t>
+  </si>
+  <si>
+    <t>Col 9</t>
+  </si>
+  <si>
+    <t>Col 10</t>
   </si>
 </sst>
 </file>
@@ -356,19 +410,20 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="B4:G23"/>
+  <dimension ref="B4:G37"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H21" activeCellId="0" sqref="H21"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A13" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D33" activeCellId="0" sqref="D33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col collapsed="false" hidden="false" max="2" min="1" style="0" width="8.53441295546559"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="0" width="29.8582995951417"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="8.53441295546559"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="14.7125506072875"/>
-    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.53441295546559"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="19.6234817813765"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="20.1740890688259"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="21.6113360323887"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.53441295546559"/>
   </cols>
   <sheetData>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -641,6 +696,90 @@
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E23" s="0" t="s">
         <v>35</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C26" s="0" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C27" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="D27" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="E27" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="F27" s="0" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B28" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="D28" s="0" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B29" s="0" t="s">
+        <v>41</v>
+      </c>
+      <c r="D29" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="E29" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="F29" s="0" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B30" s="0" t="s">
+        <v>45</v>
+      </c>
+      <c r="D30" s="0" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B31" s="0" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B32" s="0" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B33" s="0" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B34" s="0" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B35" s="0" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B36" s="0" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B37" s="0" t="s">
+        <v>53</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
assigned input for section 3 columns
</commit_message>
<xml_diff>
--- a/inputVars.xlsx
+++ b/inputVars.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="78">
   <si>
     <t>Signal Name</t>
   </si>
@@ -218,72 +218,145 @@
     </r>
   </si>
   <si>
-    <t>Section 3</t>
-  </si>
-  <si>
-    <t>operation</t>
-  </si>
-  <si>
-    <t>signal</t>
+    <t>Section 3 input columns</t>
+  </si>
+  <si>
+    <t>Operation</t>
+  </si>
+  <si>
+    <t>Signal 1</t>
+  </si>
+  <si>
+    <t>Signal 2</t>
+  </si>
+  <si>
+    <t>Signal 3</t>
+  </si>
+  <si>
+    <t>(none,  and, or)</t>
+  </si>
+  <si>
+    <t>mandatory</t>
+  </si>
+  <si>
+    <t>Only if (and, or)</t>
+  </si>
+  <si>
+    <t>Col 0</t>
+  </si>
+  <si>
+    <t>none</t>
+  </si>
+  <si>
+    <t>variable crossPercent 3</t>
   </si>
   <si>
     <t>Col 1</t>
   </si>
   <si>
-    <t>variable crossPercent 3</t>
+    <t>or</t>
+  </si>
+  <si>
+    <t>crossAbove 10 50</t>
+  </si>
+  <si>
+    <t>crossAbove 10 100</t>
+  </si>
+  <si>
+    <t>crossAbove 10 200</t>
   </si>
   <si>
     <t>Col 2</t>
   </si>
   <si>
-    <t>crossAbove 10 50</t>
-  </si>
-  <si>
-    <t>crossAbove 10 100</t>
-  </si>
-  <si>
-    <t>crossAbove 10 200</t>
+    <t>topLine 10</t>
   </si>
   <si>
     <t>Col 3</t>
   </si>
   <si>
-    <t>topLine 10</t>
+    <t>and</t>
+  </si>
+  <si>
+    <t>priceAbove 10 100</t>
+  </si>
+  <si>
+    <t>priceAbove 10 200</t>
   </si>
   <si>
     <t>Col 4</t>
   </si>
   <si>
+    <t>priceAbove 50 30</t>
+  </si>
+  <si>
     <t>Col 5</t>
   </si>
   <si>
-    <t>Col 6</t>
-  </si>
-  <si>
-    <t>Col 7</t>
-  </si>
-  <si>
-    <t>Col 8</t>
-  </si>
-  <si>
-    <t>Col 9</t>
-  </si>
-  <si>
-    <t>Col 10</t>
+    <t>Col 6*</t>
+  </si>
+  <si>
+    <t>Col 7*</t>
+  </si>
+  <si>
+    <t>Col 8*</t>
+  </si>
+  <si>
+    <t>Col 9*</t>
+  </si>
+  <si>
+    <t>* not mandatory</t>
+  </si>
+  <si>
+    <t>Section 3 input test</t>
+  </si>
+  <si>
+    <t>Column</t>
+  </si>
+  <si>
+    <t>Test 1</t>
+  </si>
+  <si>
+    <t>Part 1</t>
+  </si>
+  <si>
+    <t>Part 2</t>
+  </si>
+  <si>
+    <t>Part 3</t>
+  </si>
+  <si>
+    <t>Part 4</t>
+  </si>
+  <si>
+    <t>Part 5</t>
+  </si>
+  <si>
+    <t>Part 6</t>
+  </si>
+  <si>
+    <t>Part 7</t>
+  </si>
+  <si>
+    <t>Part 8</t>
+  </si>
+  <si>
+    <t>Test 2</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="5">
+  <numFmts count="6">
     <numFmt numFmtId="164" formatCode="GENERAL"/>
     <numFmt numFmtId="165" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* \-??_);_(@_)"/>
     <numFmt numFmtId="166" formatCode="_(* #,##0.0_);_(* \(#,##0.0\);_(* \-??_);_(@_)"/>
     <numFmt numFmtId="167" formatCode="0%"/>
     <numFmt numFmtId="168" formatCode="0.0%"/>
+    <numFmt numFmtId="169" formatCode="&quot;TRUE&quot;;&quot;TRUE&quot;;&quot;FALSE&quot;"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -308,6 +381,15 @@
     </font>
     <font>
       <b val="true"/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <u val="single"/>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
@@ -368,7 +450,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -393,6 +475,14 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
@@ -410,19 +500,19 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="B4:G37"/>
+  <dimension ref="A4:G57"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A13" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D33" activeCellId="0" sqref="D33"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A19" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C54" activeCellId="0" sqref="C54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col collapsed="false" hidden="false" max="2" min="1" style="0" width="8.53441295546559"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="29.8582995951417"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="30.9797570850202"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="0" width="19.6234817813765"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="20.1740890688259"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="21.6113360323887"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="20.9433198380567"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="21.82995951417"/>
     <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.53441295546559"/>
   </cols>
   <sheetData>
@@ -548,7 +638,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" customFormat="false" ht="15.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B11" s="0" t="s">
         <v>19</v>
       </c>
@@ -698,88 +788,218 @@
         <v>35</v>
       </c>
     </row>
+    <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C25" s="6" t="s">
+        <v>36</v>
+      </c>
+    </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C26" s="0" t="s">
-        <v>36</v>
+      <c r="C26" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="D26" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="E26" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="F26" s="4" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C27" s="0" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="D27" s="0" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="E27" s="0" t="s">
-        <v>38</v>
+        <v>43</v>
       </c>
       <c r="F27" s="0" t="s">
-        <v>38</v>
+        <v>43</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B28" s="0" t="s">
-        <v>39</v>
+        <v>44</v>
+      </c>
+      <c r="C28" s="7" t="s">
+        <v>45</v>
       </c>
       <c r="D28" s="0" t="s">
-        <v>40</v>
+        <v>46</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B29" s="0" t="s">
-        <v>41</v>
+        <v>47</v>
+      </c>
+      <c r="C29" s="0" t="s">
+        <v>48</v>
       </c>
       <c r="D29" s="0" t="s">
-        <v>42</v>
+        <v>49</v>
       </c>
       <c r="E29" s="0" t="s">
-        <v>43</v>
+        <v>50</v>
       </c>
       <c r="F29" s="0" t="s">
-        <v>44</v>
+        <v>51</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B30" s="0" t="s">
+        <v>52</v>
+      </c>
+      <c r="C30" s="0" t="s">
         <v>45</v>
       </c>
       <c r="D30" s="0" t="s">
-        <v>46</v>
+        <v>53</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B31" s="0" t="s">
-        <v>47</v>
+        <v>54</v>
+      </c>
+      <c r="C31" s="0" t="s">
+        <v>55</v>
+      </c>
+      <c r="D31" s="0" t="s">
+        <v>56</v>
+      </c>
+      <c r="E31" s="0" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B32" s="0" t="s">
-        <v>48</v>
+        <v>58</v>
+      </c>
+      <c r="C32" s="0" t="s">
+        <v>45</v>
+      </c>
+      <c r="D32" s="0" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B33" s="0" t="s">
-        <v>49</v>
+        <v>60</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B34" s="0" t="s">
-        <v>50</v>
+        <v>61</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B35" s="0" t="s">
-        <v>51</v>
+        <v>62</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B36" s="0" t="s">
-        <v>52</v>
+        <v>63</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B37" s="0" t="s">
-        <v>53</v>
+        <v>64</v>
+      </c>
+    </row>
+    <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B39" s="0" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C42" s="6" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C43" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="D43" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="E43" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="F43" s="4" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A45" s="0" t="s">
+        <v>68</v>
+      </c>
+      <c r="B45" s="0" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B46" s="0" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B47" s="0" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="48" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B48" s="0" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B49" s="0" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B50" s="0" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B51" s="0" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="52" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B52" s="0" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="53" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="54" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A54" s="0" t="s">
+        <v>77</v>
+      </c>
+      <c r="B54" s="0" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="55" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B55" s="0" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="56" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B56" s="0" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="57" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B57" s="0" t="s">
+        <v>72</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
with parameter to skip final tests
</commit_message>
<xml_diff>
--- a/inputVars.xlsx
+++ b/inputVars.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="94">
   <si>
     <t>Signal Name</t>
   </si>
@@ -233,6 +233,12 @@
     <t>Signal 3</t>
   </si>
   <si>
+    <t>Signal 4</t>
+  </si>
+  <si>
+    <t>Signal 5</t>
+  </si>
+  <si>
     <t>(none,  and, or)</t>
   </si>
   <si>
@@ -293,25 +299,43 @@
     <t>Col 5</t>
   </si>
   <si>
-    <t>Col 6*</t>
-  </si>
-  <si>
-    <t>Col 7*</t>
-  </si>
-  <si>
-    <t>Col 8*</t>
-  </si>
-  <si>
-    <t>Col 9*</t>
-  </si>
-  <si>
-    <t>* not mandatory</t>
+    <t>variable crossPercent 5</t>
+  </si>
+  <si>
+    <t>crossAbove 10 30</t>
+  </si>
+  <si>
+    <t>Col 6</t>
+  </si>
+  <si>
+    <t>Col 7</t>
+  </si>
+  <si>
+    <t>Col 8</t>
+  </si>
+  <si>
+    <t>Col 9</t>
   </si>
   <si>
     <t>Section 3 input test</t>
   </si>
   <si>
-    <t>Column</t>
+    <t>Skip Test 2</t>
+  </si>
+  <si>
+    <t>if sum (number)</t>
+  </si>
+  <si>
+    <t>Column + Days Prior</t>
+  </si>
+  <si>
+    <t>(none, sum, and, or)</t>
+  </si>
+  <si>
+    <t>(col0 – col9)  ( 0,1,2…)</t>
+  </si>
+  <si>
+    <t>(skip)</t>
   </si>
   <si>
     <t>Test 1</t>
@@ -320,9 +344,30 @@
     <t>Part 1</t>
   </si>
   <si>
+    <t>sum</t>
+  </si>
+  <si>
+    <t>col0 1</t>
+  </si>
+  <si>
+    <t>col1 1</t>
+  </si>
+  <si>
+    <t>col2 0</t>
+  </si>
+  <si>
     <t>Part 2</t>
   </si>
   <si>
+    <t>col3 0</t>
+  </si>
+  <si>
+    <t>col4 0</t>
+  </si>
+  <si>
+    <t>col5 0</t>
+  </si>
+  <si>
     <t>Part 3</t>
   </si>
   <si>
@@ -338,10 +383,13 @@
     <t>Part 7</t>
   </si>
   <si>
-    <t>Part 8</t>
-  </si>
-  <si>
     <t>Test 2</t>
+  </si>
+  <si>
+    <t>Col5 0</t>
+  </si>
+  <si>
+    <t>FinalTest Number of Days Return</t>
   </si>
 </sst>
 </file>
@@ -500,10 +548,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A4:G57"/>
+  <dimension ref="A4:X60"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A19" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C54" activeCellId="0" sqref="C54"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="M37" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="O53" activeCellId="0" sqref="O53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -511,9 +559,12 @@
     <col collapsed="false" hidden="false" max="2" min="1" style="0" width="8.53441295546559"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="0" width="30.9797570850202"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="0" width="19.6234817813765"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="20.9433198380567"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="21.82995951417"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.53441295546559"/>
+    <col collapsed="false" hidden="false" max="14" min="5" style="0" width="20.3967611336032"/>
+    <col collapsed="false" hidden="false" max="16" min="15" style="0" width="20.502024291498"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="18.080971659919"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="19.0728744939271"/>
+    <col collapsed="false" hidden="false" max="24" min="19" style="0" width="19.7327935222672"/>
+    <col collapsed="false" hidden="false" max="1025" min="25" style="0" width="8.53441295546559"/>
   </cols>
   <sheetData>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -806,200 +857,373 @@
       <c r="F26" s="4" t="s">
         <v>40</v>
       </c>
+      <c r="G26" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="H26" s="4" t="s">
+        <v>42</v>
+      </c>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C27" s="0" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="D27" s="0" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="E27" s="0" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="F27" s="0" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B28" s="0" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="C28" s="7" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="D28" s="0" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B29" s="0" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="C29" s="0" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="D29" s="0" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="E29" s="0" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="F29" s="0" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B30" s="0" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="C30" s="0" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="D30" s="0" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B31" s="0" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="C31" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="D31" s="0" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="E31" s="0" t="s">
-        <v>57</v>
+        <v>59</v>
+      </c>
+      <c r="F31" s="0" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B32" s="0" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="C32" s="0" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="D32" s="0" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B33" s="0" t="s">
-        <v>60</v>
+        <v>62</v>
+      </c>
+      <c r="C33" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="D33" s="0" t="s">
+        <v>63</v>
+      </c>
+      <c r="E33" s="0" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B34" s="0" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B35" s="0" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B36" s="0" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B37" s="0" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B39" s="0" t="s">
-        <v>65</v>
-      </c>
-    </row>
+        <v>68</v>
+      </c>
+    </row>
+    <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C42" s="6" t="s">
-        <v>66</v>
+        <v>69</v>
+      </c>
+      <c r="E42" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F42" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="G42" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="H42" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="I42" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="J42" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="K42" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="L42" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="M42" s="0" t="n">
+        <v>9</v>
+      </c>
+      <c r="N42" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="O42" s="4" t="s">
+        <v>70</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C43" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="D43" s="4" t="s">
-        <v>67</v>
+      <c r="D43" s="0" t="s">
+        <v>71</v>
       </c>
       <c r="E43" s="4" t="s">
-        <v>67</v>
+        <v>72</v>
       </c>
       <c r="F43" s="4" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+        <v>72</v>
+      </c>
+      <c r="G43" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="H43" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="I43" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="J43" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="K43" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="L43" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="M43" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="N43" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="O43" s="1"/>
+      <c r="P43" s="4"/>
+      <c r="Q43" s="4"/>
+      <c r="R43" s="4"/>
+      <c r="S43" s="4"/>
+      <c r="T43" s="4"/>
+      <c r="U43" s="4"/>
+      <c r="V43" s="4"/>
+      <c r="W43" s="4"/>
+      <c r="X43" s="4"/>
+    </row>
+    <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C44" s="0" t="s">
+        <v>73</v>
+      </c>
+      <c r="E44" s="0" t="s">
+        <v>74</v>
+      </c>
+      <c r="F44" s="0" t="s">
+        <v>74</v>
+      </c>
+      <c r="G44" s="0" t="s">
+        <v>74</v>
+      </c>
+      <c r="H44" s="0" t="s">
+        <v>74</v>
+      </c>
+      <c r="I44" s="0" t="s">
+        <v>74</v>
+      </c>
+      <c r="J44" s="0" t="s">
+        <v>74</v>
+      </c>
+      <c r="K44" s="0" t="s">
+        <v>74</v>
+      </c>
+      <c r="L44" s="0" t="s">
+        <v>74</v>
+      </c>
+      <c r="M44" s="0" t="s">
+        <v>74</v>
+      </c>
+      <c r="N44" s="0" t="s">
+        <v>74</v>
+      </c>
+      <c r="O44" s="0" t="s">
+        <v>75</v>
+      </c>
+    </row>
     <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="0" t="s">
-        <v>68</v>
+        <v>76</v>
       </c>
       <c r="B45" s="0" t="s">
-        <v>69</v>
+        <v>77</v>
+      </c>
+      <c r="C45" s="0" t="s">
+        <v>78</v>
+      </c>
+      <c r="D45" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="E45" s="0" t="s">
+        <v>79</v>
+      </c>
+      <c r="F45" s="0" t="s">
+        <v>80</v>
+      </c>
+      <c r="G45" s="0" t="s">
+        <v>81</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B46" s="0" t="s">
-        <v>70</v>
+        <v>82</v>
+      </c>
+      <c r="C46" s="0" t="s">
+        <v>57</v>
+      </c>
+      <c r="E46" s="0" t="s">
+        <v>83</v>
+      </c>
+      <c r="F46" s="0" t="s">
+        <v>84</v>
+      </c>
+      <c r="G46" s="0" t="s">
+        <v>85</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B47" s="0" t="s">
-        <v>71</v>
+        <v>86</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B48" s="0" t="s">
-        <v>72</v>
+        <v>87</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B49" s="0" t="s">
-        <v>73</v>
+        <v>88</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B50" s="0" t="s">
-        <v>74</v>
+        <v>89</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B51" s="0" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="52" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B52" s="0" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="53" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+        <v>90</v>
+      </c>
+    </row>
+    <row r="52" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="53" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="O53" s="0" t="s">
+        <v>70</v>
+      </c>
+    </row>
     <row r="54" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="0" t="s">
+        <v>91</v>
+      </c>
+      <c r="B54" s="0" t="s">
         <v>77</v>
       </c>
-      <c r="B54" s="0" t="s">
-        <v>69</v>
+      <c r="C54" s="0" t="s">
+        <v>47</v>
+      </c>
+      <c r="E54" s="0" t="s">
+        <v>84</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B55" s="0" t="s">
-        <v>70</v>
+        <v>82</v>
+      </c>
+      <c r="C55" s="0" t="s">
+        <v>47</v>
+      </c>
+      <c r="E55" s="0" t="s">
+        <v>92</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B56" s="0" t="s">
-        <v>71</v>
+        <v>86</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B57" s="0" t="s">
-        <v>72</v>
+        <v>87</v>
+      </c>
+    </row>
+    <row r="58" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B58" s="0" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="60" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C60" s="0" t="s">
+        <v>93</v>
+      </c>
+      <c r="D60" s="0" t="n">
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
with return stats and formated decently well
</commit_message>
<xml_diff>
--- a/inputVars.xlsx
+++ b/inputVars.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="96">
   <si>
     <t>Signal Name</t>
   </si>
@@ -320,15 +320,15 @@
     <t>Section 3 input test</t>
   </si>
   <si>
+    <t>if sum (number)</t>
+  </si>
+  <si>
+    <t>Column + Days Prior</t>
+  </si>
+  <si>
     <t>Skip Test 2</t>
   </si>
   <si>
-    <t>if sum (number)</t>
-  </si>
-  <si>
-    <t>Column + Days Prior</t>
-  </si>
-  <si>
     <t>(none, sum, and, or)</t>
   </si>
   <si>
@@ -368,6 +368,9 @@
     <t>col5 0</t>
   </si>
   <si>
+    <t>skip</t>
+  </si>
+  <si>
     <t>Part 3</t>
   </si>
   <si>
@@ -381,6 +384,21 @@
   </si>
   <si>
     <t>Part 7</t>
+  </si>
+  <si>
+    <r>
+      <t>Skip Test 1 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t>(skip)</t>
+    </r>
   </si>
   <si>
     <t>Test 2</t>
@@ -550,8 +568,8 @@
   </sheetPr>
   <dimension ref="A4:X60"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="M37" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="O53" activeCellId="0" sqref="O53"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="G22" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="O46" activeCellId="0" sqref="O46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1017,48 +1035,47 @@
       <c r="N42" s="0" t="n">
         <v>10</v>
       </c>
-      <c r="O42" s="4" t="s">
-        <v>70</v>
-      </c>
     </row>
     <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C43" s="4" t="s">
         <v>37</v>
       </c>
       <c r="D43" s="0" t="s">
+        <v>70</v>
+      </c>
+      <c r="E43" s="4" t="s">
         <v>71</v>
       </c>
-      <c r="E43" s="4" t="s">
+      <c r="F43" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="G43" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="H43" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="I43" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="J43" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="K43" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="L43" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="M43" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="N43" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="O43" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="F43" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="G43" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="H43" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="I43" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="J43" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="K43" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="L43" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="M43" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="N43" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="O43" s="1"/>
       <c r="P43" s="4"/>
       <c r="Q43" s="4"/>
       <c r="R43" s="4"/>
@@ -1146,41 +1163,44 @@
       <c r="G46" s="0" t="s">
         <v>85</v>
       </c>
+      <c r="O46" s="0" t="s">
+        <v>86</v>
+      </c>
     </row>
     <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B47" s="0" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B48" s="0" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B49" s="0" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B50" s="0" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B51" s="0" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="53" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O53" s="0" t="s">
-        <v>70</v>
+    <row r="53" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="O53" s="4" t="s">
+        <v>92</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="0" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="B54" s="0" t="s">
         <v>77</v>
@@ -1200,30 +1220,30 @@
         <v>47</v>
       </c>
       <c r="E55" s="0" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B56" s="0" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B57" s="0" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B58" s="0" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C60" s="0" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="D60" s="0" t="n">
-        <v>20</v>
+        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>